<commit_message>
Feature/thpds  project coding (#2060)
* support OUVP Component

* Update Config File

* Support CB -> RCD

Co-authored-by: THAPE\tiankaihe <1204973192@qq.com>
</commit_message>
<xml_diff>
--- a/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_OUVP_19DX101.xlsx
+++ b/AutoLoader/Contents/Support/PowerDistributionSystem/LV_AC_OUVP_19DX101.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C07A2D1-DA15-42A1-9B43-D1ACC1EF6198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="-132" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-132" windowWidth="30936" windowHeight="16896"/>
   </bookViews>
   <sheets>
-    <sheet name="CJ20" sheetId="1" r:id="rId1"/>
+    <sheet name="OUVP" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -105,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,11 +428,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>